<commit_message>
updates to warm ups
</commit_message>
<xml_diff>
--- a/Semester2/grades/Grades.xlsx
+++ b/Semester2/grades/Grades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">Homework 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homework 2</t>
   </si>
   <si>
     <t xml:space="preserve">Susana</t>
@@ -284,10 +287,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -296,7 +299,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.11"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="8.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="8.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -314,245 +319,312 @@
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F3" s="1" t="n">
         <f aca="false">10.5/10</f>
         <v>1.05</v>
       </c>
+      <c r="G3" s="1" t="n">
+        <f aca="false">10.5/12</f>
+        <v>0.875</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
+      <c r="G4" s="1" t="n">
+        <f aca="false">6/12</f>
+        <v>0.5</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" s="1" t="n">
         <f aca="false">9.25/10</f>
         <v>0.925</v>
       </c>
+      <c r="G5" s="1" t="n">
+        <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F6" s="1" t="n">
         <f aca="false">9.75/10</f>
         <v>0.975</v>
       </c>
+      <c r="G6" s="1" t="n">
+        <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" s="1" t="n">
         <f aca="false">9.75/10</f>
         <v>0.975</v>
       </c>
+      <c r="G7" s="1" t="n">
+        <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F8" s="1" t="n">
         <f aca="false">8/10</f>
         <v>0.8</v>
       </c>
+      <c r="G8" s="1" t="n">
+        <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F9" s="1" t="n">
         <f aca="false">8/10</f>
         <v>0.8</v>
       </c>
+      <c r="G9" s="1" t="n">
+        <f aca="false">10/12</f>
+        <v>0.833333333333333</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F11" s="1" t="n">
         <f aca="false">9.5/10</f>
         <v>0.95</v>
       </c>
+      <c r="G11" s="1" t="n">
+        <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F12" s="1" t="n">
         <f aca="false">8.5/10</f>
         <v>0.85</v>
       </c>
+      <c r="G12" s="1" t="n">
+        <f aca="false">11/12</f>
+        <v>0.916666666666667</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F13" s="1" t="n">
         <f aca="false">9.5/10</f>
         <v>0.95</v>
       </c>
+      <c r="G13" s="1" t="n">
+        <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F14" s="1" t="n">
         <f aca="false">9.5/10</f>
         <v>0.95</v>
       </c>
+      <c r="G14" s="1" t="n">
+        <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F15" s="1" t="n">
         <f aca="false">9.75/10</f>
         <v>0.975</v>
       </c>
+      <c r="G15" s="1" t="n">
+        <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F16" s="1" t="n">
         <f aca="false">9/10</f>
         <v>0.9</v>
       </c>
+      <c r="G16" s="1" t="n">
+        <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">9/10</f>
         <v>0.9</v>
       </c>
+      <c r="G17" s="1" t="n">
+        <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">9.5/10</f>
         <v>0.95</v>
       </c>
+      <c r="G18" s="1" t="n">
+        <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">9/10</f>
         <v>0.9</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <f aca="false">12/12</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
graded a homework and updated a reading quiz
</commit_message>
<xml_diff>
--- a/Semester2/grades/Grades.xlsx
+++ b/Semester2/grades/Grades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">Homework 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homework 3</t>
   </si>
   <si>
     <t xml:space="preserve">Susana</t>
@@ -287,10 +290,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -301,7 +304,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.91"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="8.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -322,16 +326,19 @@
       <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F3" s="1" t="n">
         <f aca="false">10.5/10</f>
@@ -341,16 +348,20 @@
         <f aca="false">10.5/12</f>
         <v>0.875</v>
       </c>
+      <c r="H3" s="1" t="n">
+        <f aca="false">14/13</f>
+        <v>1.07692307692308</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1" t="n">
         <f aca="false">0</f>
@@ -360,16 +371,20 @@
         <f aca="false">6/12</f>
         <v>0.5</v>
       </c>
+      <c r="H4" s="1" t="n">
+        <f aca="false">8/13</f>
+        <v>0.615384615384615</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="1" t="n">
         <f aca="false">9.25/10</f>
@@ -382,13 +397,13 @@
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F6" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -398,16 +413,20 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="H6" s="1" t="n">
+        <f aca="false">14/13</f>
+        <v>1.07692307692308</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F7" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -417,16 +436,20 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="H7" s="1" t="n">
+        <f aca="false">13/13</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F8" s="1" t="n">
         <f aca="false">8/10</f>
@@ -436,16 +459,20 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="H8" s="1" t="n">
+        <f aca="false">13/13</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F9" s="1" t="n">
         <f aca="false">8/10</f>
@@ -455,16 +482,20 @@
         <f aca="false">10/12</f>
         <v>0.833333333333333</v>
       </c>
+      <c r="H9" s="1" t="n">
+        <f aca="false">12/13</f>
+        <v>0.923076923076923</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F11" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -474,16 +505,20 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="H11" s="1" t="n">
+        <f aca="false">13/13</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F12" s="1" t="n">
         <f aca="false">8.5/10</f>
@@ -493,16 +528,20 @@
         <f aca="false">11/12</f>
         <v>0.916666666666667</v>
       </c>
+      <c r="H12" s="1" t="n">
+        <f aca="false">12.5/13</f>
+        <v>0.961538461538462</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F13" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -512,16 +551,20 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="H13" s="1" t="n">
+        <f aca="false">13/13</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F14" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -531,16 +574,20 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="H14" s="1" t="n">
+        <f aca="false">13/13</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F15" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -550,16 +597,20 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="H15" s="1" t="n">
+        <f aca="false">12.5/13</f>
+        <v>0.961538461538462</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F16" s="1" t="n">
         <f aca="false">9/10</f>
@@ -569,16 +620,20 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="H16" s="1" t="n">
+        <f aca="false">13/13</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">9/10</f>
@@ -588,16 +643,20 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="H17" s="1" t="n">
+        <f aca="false">13/13</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -607,16 +666,20 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="H18" s="1" t="n">
+        <f aca="false">13/13</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">9/10</f>
@@ -624,6 +687,10 @@
       </c>
       <c r="G19" s="1" t="n">
         <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <f aca="false">13/13</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated grades, reading quiz (unit 3), and midterm study guide
</commit_message>
<xml_diff>
--- a/Semester2/grades/Grades.xlsx
+++ b/Semester2/grades/Grades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">Homework 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homework 4</t>
   </si>
   <si>
     <t xml:space="preserve">Susana</t>
@@ -290,10 +293,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -305,7 +308,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.91"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.21"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="8.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -329,16 +333,19 @@
       <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1" t="n">
         <f aca="false">10.5/10</f>
@@ -352,16 +359,20 @@
         <f aca="false">14/13</f>
         <v>1.07692307692308</v>
       </c>
+      <c r="I3" s="1" t="n">
+        <f aca="false">10/10</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="n">
         <f aca="false">0</f>
@@ -375,16 +386,20 @@
         <f aca="false">8/13</f>
         <v>0.615384615384615</v>
       </c>
+      <c r="I4" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F5" s="1" t="n">
         <f aca="false">9.25/10</f>
@@ -394,16 +409,20 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="I5" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F6" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -417,16 +436,20 @@
         <f aca="false">14/13</f>
         <v>1.07692307692308</v>
       </c>
+      <c r="I6" s="1" t="n">
+        <f aca="false">11/10</f>
+        <v>1.1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F7" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -440,16 +463,20 @@
         <f aca="false">13/13</f>
         <v>1</v>
       </c>
+      <c r="I7" s="1" t="n">
+        <f aca="false">10.5/10</f>
+        <v>1.05</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="1" t="n">
         <f aca="false">8/10</f>
@@ -463,16 +490,20 @@
         <f aca="false">13/13</f>
         <v>1</v>
       </c>
+      <c r="I8" s="1" t="n">
+        <f aca="false">10/10</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F9" s="1" t="n">
         <f aca="false">8/10</f>
@@ -486,16 +517,20 @@
         <f aca="false">12/13</f>
         <v>0.923076923076923</v>
       </c>
+      <c r="I9" s="1" t="n">
+        <f aca="false">9.5/10</f>
+        <v>0.95</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F11" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -509,16 +544,20 @@
         <f aca="false">13/13</f>
         <v>1</v>
       </c>
+      <c r="I11" s="1" t="n">
+        <f aca="false">10/10</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F12" s="1" t="n">
         <f aca="false">8.5/10</f>
@@ -532,16 +571,20 @@
         <f aca="false">12.5/13</f>
         <v>0.961538461538462</v>
       </c>
+      <c r="I12" s="1" t="n">
+        <f aca="false">9/10</f>
+        <v>0.9</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F13" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -555,16 +598,20 @@
         <f aca="false">13/13</f>
         <v>1</v>
       </c>
+      <c r="I13" s="1" t="n">
+        <f aca="false">11/10</f>
+        <v>1.1</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F14" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -578,16 +625,20 @@
         <f aca="false">13/13</f>
         <v>1</v>
       </c>
+      <c r="I14" s="1" t="n">
+        <f aca="false">9/10</f>
+        <v>0.9</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F15" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -601,16 +652,20 @@
         <f aca="false">12.5/13</f>
         <v>0.961538461538462</v>
       </c>
+      <c r="I15" s="1" t="n">
+        <f aca="false">8.5/10</f>
+        <v>0.85</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F16" s="1" t="n">
         <f aca="false">9/10</f>
@@ -624,16 +679,20 @@
         <f aca="false">13/13</f>
         <v>1</v>
       </c>
+      <c r="I16" s="1" t="n">
+        <f aca="false">10/10</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">9/10</f>
@@ -647,16 +706,20 @@
         <f aca="false">13/13</f>
         <v>1</v>
       </c>
+      <c r="I17" s="1" t="n">
+        <f aca="false">9.5/10</f>
+        <v>0.95</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -670,16 +733,20 @@
         <f aca="false">13/13</f>
         <v>1</v>
       </c>
+      <c r="I18" s="1" t="n">
+        <f aca="false">11/10</f>
+        <v>1.1</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">9/10</f>
@@ -691,6 +758,10 @@
       </c>
       <c r="H19" s="1" t="n">
         <f aca="false">13/13</f>
+        <v>1</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <f aca="false">10/10</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
starting the midterm 1 grading process
</commit_message>
<xml_diff>
--- a/Semester2/grades/Grades.xlsx
+++ b/Semester2/grades/Grades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t xml:space="preserve">Homework 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homework 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Midterm 1</t>
   </si>
   <si>
     <t xml:space="preserve">Susana</t>
@@ -293,10 +299,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -309,7 +315,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.49"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="1" width="8.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -336,16 +344,22 @@
       <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1" t="n">
         <f aca="false">10.5/10</f>
@@ -366,13 +380,13 @@
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1" t="n">
         <f aca="false">0</f>
@@ -393,13 +407,13 @@
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F5" s="1" t="n">
         <f aca="false">9.25/10</f>
@@ -416,13 +430,13 @@
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F6" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -443,13 +457,13 @@
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F7" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -470,13 +484,13 @@
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F8" s="1" t="n">
         <f aca="false">8/10</f>
@@ -497,13 +511,13 @@
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F9" s="1" t="n">
         <f aca="false">8/10</f>
@@ -524,13 +538,13 @@
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F11" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -551,13 +565,13 @@
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F12" s="1" t="n">
         <f aca="false">8.5/10</f>
@@ -578,13 +592,13 @@
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F13" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -602,16 +616,20 @@
         <f aca="false">11/10</f>
         <v>1.1</v>
       </c>
+      <c r="K13" s="1" t="n">
+        <f aca="false">44/50</f>
+        <v>0.88</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F14" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -632,13 +650,13 @@
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F15" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -656,16 +674,20 @@
         <f aca="false">8.5/10</f>
         <v>0.85</v>
       </c>
+      <c r="K15" s="1" t="n">
+        <f aca="false">46/50</f>
+        <v>0.92</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F16" s="1" t="n">
         <f aca="false">9/10</f>
@@ -686,13 +708,13 @@
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">9/10</f>
@@ -713,13 +735,13 @@
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -740,13 +762,13 @@
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">9/10</f>

</xml_diff>

<commit_message>
midterm 1 grading completed, minus late submissions
</commit_message>
<xml_diff>
--- a/Semester2/grades/Grades.xlsx
+++ b/Semester2/grades/Grades.xlsx
@@ -302,7 +302,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
+      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -377,6 +377,10 @@
         <f aca="false">10/10</f>
         <v>1</v>
       </c>
+      <c r="K3" s="1" t="n">
+        <f aca="false">47/50</f>
+        <v>0.94</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -404,6 +408,10 @@
         <f aca="false">0</f>
         <v>0</v>
       </c>
+      <c r="K4" s="1" t="n">
+        <f aca="false">31/50</f>
+        <v>0.62</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -427,6 +435,10 @@
         <f aca="false">0</f>
         <v>0</v>
       </c>
+      <c r="K5" s="1" t="n">
+        <f aca="false">43/50</f>
+        <v>0.86</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -454,6 +466,10 @@
         <f aca="false">11/10</f>
         <v>1.1</v>
       </c>
+      <c r="K6" s="1" t="n">
+        <f aca="false">46.5/50</f>
+        <v>0.93</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -481,6 +497,10 @@
         <f aca="false">10.5/10</f>
         <v>1.05</v>
       </c>
+      <c r="K7" s="1" t="n">
+        <f aca="false">43/50</f>
+        <v>0.86</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -508,6 +528,9 @@
         <f aca="false">10/10</f>
         <v>1</v>
       </c>
+      <c r="K8" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -535,6 +558,9 @@
         <f aca="false">9.5/10</f>
         <v>0.95</v>
       </c>
+      <c r="K9" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -562,6 +588,10 @@
         <f aca="false">10/10</f>
         <v>1</v>
       </c>
+      <c r="K11" s="1" t="n">
+        <f aca="false">41/50</f>
+        <v>0.82</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -589,6 +619,10 @@
         <f aca="false">9/10</f>
         <v>0.9</v>
       </c>
+      <c r="K12" s="1" t="n">
+        <f aca="false">42/50</f>
+        <v>0.84</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -647,6 +681,10 @@
         <f aca="false">9/10</f>
         <v>0.9</v>
       </c>
+      <c r="K14" s="1" t="n">
+        <f aca="false">37.5/50</f>
+        <v>0.75</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
@@ -705,6 +743,10 @@
         <f aca="false">10/10</f>
         <v>1</v>
       </c>
+      <c r="K16" s="1" t="n">
+        <f aca="false">47/50</f>
+        <v>0.94</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
@@ -732,6 +774,10 @@
         <f aca="false">9.5/10</f>
         <v>0.95</v>
       </c>
+      <c r="K17" s="1" t="n">
+        <f aca="false">45.5/50</f>
+        <v>0.91</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -759,6 +805,10 @@
         <f aca="false">11/10</f>
         <v>1.1</v>
       </c>
+      <c r="K18" s="1" t="n">
+        <f aca="false">42/50</f>
+        <v>0.84</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -785,6 +835,10 @@
       <c r="I19" s="1" t="n">
         <f aca="false">10/10</f>
         <v>1</v>
+      </c>
+      <c r="K19" s="1" t="n">
+        <f aca="false">45.5/50</f>
+        <v>0.91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding grades to midterm 1 and updating reading quizzes
</commit_message>
<xml_diff>
--- a/Semester2/grades/Grades.xlsx
+++ b/Semester2/grades/Grades.xlsx
@@ -302,7 +302,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
+      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -682,8 +682,8 @@
         <v>0.9</v>
       </c>
       <c r="K14" s="1" t="n">
-        <f aca="false">37.5/50</f>
-        <v>0.75</v>
+        <f aca="false">40/50</f>
+        <v>0.8</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
grading homework 5 and reading quiz updates
</commit_message>
<xml_diff>
--- a/Semester2/grades/Grades.xlsx
+++ b/Semester2/grades/Grades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">Midterm 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homework 6</t>
   </si>
   <si>
     <t xml:space="preserve">Susana</t>
@@ -299,10 +302,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
+      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -317,7 +320,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.49"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="1" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="13" style="1" width="8.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -350,16 +354,19 @@
       <c r="K2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="L2" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="n">
         <f aca="false">10.5/10</f>
@@ -377,6 +384,10 @@
         <f aca="false">10/10</f>
         <v>1</v>
       </c>
+      <c r="J3" s="1" t="n">
+        <f aca="false">13/13</f>
+        <v>1</v>
+      </c>
       <c r="K3" s="1" t="n">
         <f aca="false">47/50</f>
         <v>0.94</v>
@@ -384,13 +395,13 @@
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1" t="n">
         <f aca="false">0</f>
@@ -408,6 +419,9 @@
         <f aca="false">0</f>
         <v>0</v>
       </c>
+      <c r="J4" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="K4" s="1" t="n">
         <f aca="false">31/50</f>
         <v>0.62</v>
@@ -415,13 +429,13 @@
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F5" s="1" t="n">
         <f aca="false">9.25/10</f>
@@ -435,6 +449,10 @@
         <f aca="false">0</f>
         <v>0</v>
       </c>
+      <c r="J5" s="1" t="n">
+        <f aca="false">13/13</f>
+        <v>1</v>
+      </c>
       <c r="K5" s="1" t="n">
         <f aca="false">43/50</f>
         <v>0.86</v>
@@ -442,13 +460,13 @@
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F6" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -466,6 +484,10 @@
         <f aca="false">11/10</f>
         <v>1.1</v>
       </c>
+      <c r="J6" s="1" t="n">
+        <f aca="false">12.5/13</f>
+        <v>0.961538461538462</v>
+      </c>
       <c r="K6" s="1" t="n">
         <f aca="false">46.5/50</f>
         <v>0.93</v>
@@ -473,13 +495,13 @@
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -497,6 +519,10 @@
         <f aca="false">10.5/10</f>
         <v>1.05</v>
       </c>
+      <c r="J7" s="1" t="n">
+        <f aca="false">12.5/13</f>
+        <v>0.961538461538462</v>
+      </c>
       <c r="K7" s="1" t="n">
         <f aca="false">43/50</f>
         <v>0.86</v>
@@ -504,13 +530,13 @@
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F8" s="1" t="n">
         <f aca="false">8/10</f>
@@ -528,19 +554,23 @@
         <f aca="false">10/10</f>
         <v>1</v>
       </c>
+      <c r="J8" s="1" t="n">
+        <f aca="false">11/13</f>
+        <v>0.846153846153846</v>
+      </c>
       <c r="K8" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F9" s="1" t="n">
         <f aca="false">8/10</f>
@@ -558,19 +588,23 @@
         <f aca="false">9.5/10</f>
         <v>0.95</v>
       </c>
+      <c r="J9" s="1" t="n">
+        <f aca="false">13/13</f>
+        <v>1</v>
+      </c>
       <c r="K9" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F11" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -588,6 +622,10 @@
         <f aca="false">10/10</f>
         <v>1</v>
       </c>
+      <c r="J11" s="1" t="n">
+        <f aca="false">13/13</f>
+        <v>1</v>
+      </c>
       <c r="K11" s="1" t="n">
         <f aca="false">41/50</f>
         <v>0.82</v>
@@ -595,13 +633,13 @@
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F12" s="1" t="n">
         <f aca="false">8.5/10</f>
@@ -619,6 +657,10 @@
         <f aca="false">9/10</f>
         <v>0.9</v>
       </c>
+      <c r="J12" s="1" t="n">
+        <f aca="false">12/13</f>
+        <v>0.923076923076923</v>
+      </c>
       <c r="K12" s="1" t="n">
         <f aca="false">42/50</f>
         <v>0.84</v>
@@ -626,13 +668,13 @@
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F13" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -650,6 +692,10 @@
         <f aca="false">11/10</f>
         <v>1.1</v>
       </c>
+      <c r="J13" s="1" t="n">
+        <f aca="false">13/13</f>
+        <v>1</v>
+      </c>
       <c r="K13" s="1" t="n">
         <f aca="false">44/50</f>
         <v>0.88</v>
@@ -657,13 +703,13 @@
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F14" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -681,6 +727,10 @@
         <f aca="false">9/10</f>
         <v>0.9</v>
       </c>
+      <c r="J14" s="1" t="n">
+        <f aca="false">13/13</f>
+        <v>1</v>
+      </c>
       <c r="K14" s="1" t="n">
         <f aca="false">40/50</f>
         <v>0.8</v>
@@ -688,13 +738,13 @@
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F15" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -712,6 +762,10 @@
         <f aca="false">8.5/10</f>
         <v>0.85</v>
       </c>
+      <c r="J15" s="1" t="n">
+        <f aca="false">13/13</f>
+        <v>1</v>
+      </c>
       <c r="K15" s="1" t="n">
         <f aca="false">46/50</f>
         <v>0.92</v>
@@ -719,13 +773,13 @@
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F16" s="1" t="n">
         <f aca="false">9/10</f>
@@ -743,6 +797,10 @@
         <f aca="false">10/10</f>
         <v>1</v>
       </c>
+      <c r="J16" s="1" t="n">
+        <f aca="false">13/13</f>
+        <v>1</v>
+      </c>
       <c r="K16" s="1" t="n">
         <f aca="false">47/50</f>
         <v>0.94</v>
@@ -750,13 +808,13 @@
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">9/10</f>
@@ -774,6 +832,10 @@
         <f aca="false">9.5/10</f>
         <v>0.95</v>
       </c>
+      <c r="J17" s="1" t="n">
+        <f aca="false">13/13</f>
+        <v>1</v>
+      </c>
       <c r="K17" s="1" t="n">
         <f aca="false">45.5/50</f>
         <v>0.91</v>
@@ -781,13 +843,13 @@
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -812,13 +874,13 @@
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">9/10</f>
@@ -834,6 +896,10 @@
       </c>
       <c r="I19" s="1" t="n">
         <f aca="false">10/10</f>
+        <v>1</v>
+      </c>
+      <c r="J19" s="1" t="n">
+        <f aca="false">13/13</f>
         <v>1</v>
       </c>
       <c r="K19" s="1" t="n">

</xml_diff>

<commit_message>
more grading, reading quiz
</commit_message>
<xml_diff>
--- a/Semester2/grades/Grades.xlsx
+++ b/Semester2/grades/Grades.xlsx
@@ -304,8 +304,8 @@
   </sheetPr>
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -593,7 +593,8 @@
         <v>1</v>
       </c>
       <c r="K9" s="1" t="n">
-        <v>0</v>
+        <f aca="false">45/50</f>
+        <v>0.9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updates: reading quizzes, grading, some figures, lecture note typos
</commit_message>
<xml_diff>
--- a/Semester2/grades/Grades.xlsx
+++ b/Semester2/grades/Grades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">Homework 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final Project Proposal</t>
   </si>
   <si>
     <t xml:space="preserve">Susana</t>
@@ -302,10 +305,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
+      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -321,7 +324,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.71"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="13" style="1" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="21.48"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="1" width="8.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -357,16 +361,19 @@
       <c r="L2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="M2" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="n">
         <f aca="false">10.5/10</f>
@@ -399,13 +406,13 @@
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" s="1" t="n">
         <f aca="false">0</f>
@@ -437,13 +444,13 @@
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1" t="n">
         <f aca="false">9.25/10</f>
@@ -472,13 +479,13 @@
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -511,13 +518,13 @@
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F7" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -550,13 +557,13 @@
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" s="1" t="n">
         <f aca="false">8/10</f>
@@ -579,7 +586,8 @@
         <v>0.846153846153846</v>
       </c>
       <c r="K8" s="1" t="n">
-        <v>0</v>
+        <f aca="false">45/50</f>
+        <v>0.9</v>
       </c>
       <c r="L8" s="1" t="n">
         <f aca="false">11/12</f>
@@ -588,13 +596,13 @@
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F9" s="1" t="n">
         <f aca="false">8/10</f>
@@ -627,13 +635,13 @@
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F11" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -663,16 +671,19 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="M11" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F12" s="1" t="n">
         <f aca="false">8.5/10</f>
@@ -705,13 +716,13 @@
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F13" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -741,16 +752,19 @@
         <f aca="false">11.5/12</f>
         <v>0.958333333333333</v>
       </c>
+      <c r="M13" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F14" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -780,16 +794,19 @@
         <f aca="false">11/12</f>
         <v>0.916666666666667</v>
       </c>
+      <c r="M14" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F15" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -819,16 +836,19 @@
         <f aca="false">11/12</f>
         <v>0.916666666666667</v>
       </c>
+      <c r="M15" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F16" s="1" t="n">
         <f aca="false">9/10</f>
@@ -861,13 +881,13 @@
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">9/10</f>
@@ -900,13 +920,13 @@
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -932,16 +952,19 @@
         <f aca="false">11.5/12</f>
         <v>0.958333333333333</v>
       </c>
+      <c r="M18" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">9/10</f>

</xml_diff>

<commit_message>
many reading quiz updates, grade updates, and midterm study guide and solutions
</commit_message>
<xml_diff>
--- a/Semester2/grades/Grades.xlsx
+++ b/Semester2/grades/Grades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t xml:space="preserve">Final Project Proposal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homework 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Midterm 2</t>
   </si>
   <si>
     <t xml:space="preserve">Susana</t>
@@ -305,10 +311,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
+      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -325,7 +331,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="21.48"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="1" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.39"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="1" width="8.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -364,16 +372,22 @@
       <c r="M2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="N2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1" t="n">
         <f aca="false">10.5/10</f>
@@ -403,16 +417,19 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="M3" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="n">
         <f aca="false">0</f>
@@ -441,16 +458,19 @@
         <f aca="false">10/12</f>
         <v>0.833333333333333</v>
       </c>
+      <c r="M4" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="n">
         <f aca="false">9.25/10</f>
@@ -460,6 +480,10 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="H5" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
       <c r="I5" s="1" t="n">
         <f aca="false">0</f>
         <v>0</v>
@@ -476,16 +500,19 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="M5" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -515,16 +542,19 @@
         <f aca="false">11/12</f>
         <v>0.916666666666667</v>
       </c>
+      <c r="M6" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F7" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -554,16 +584,19 @@
         <f aca="false">11/12</f>
         <v>0.916666666666667</v>
       </c>
+      <c r="M7" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F8" s="1" t="n">
         <f aca="false">8/10</f>
@@ -593,16 +626,19 @@
         <f aca="false">11/12</f>
         <v>0.916666666666667</v>
       </c>
+      <c r="M8" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F9" s="1" t="n">
         <f aca="false">8/10</f>
@@ -632,16 +668,19 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="M9" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F11" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -677,13 +716,13 @@
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F12" s="1" t="n">
         <f aca="false">8.5/10</f>
@@ -713,16 +752,19 @@
         <f aca="false">11/12</f>
         <v>0.916666666666667</v>
       </c>
+      <c r="M12" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F13" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -758,13 +800,13 @@
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F14" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -800,13 +842,13 @@
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F15" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -842,13 +884,13 @@
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F16" s="1" t="n">
         <f aca="false">9/10</f>
@@ -878,16 +920,19 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="M16" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">9/10</f>
@@ -917,16 +962,19 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="M17" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -958,13 +1006,13 @@
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">9/10</f>
@@ -992,6 +1040,9 @@
       </c>
       <c r="L19" s="1" t="n">
         <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
+      <c r="M19" s="1" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished grading ps 7, added midterm study guide 2 solutions
</commit_message>
<xml_diff>
--- a/Semester2/grades/Grades.xlsx
+++ b/Semester2/grades/Grades.xlsx
@@ -314,7 +314,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
+      <selection pane="topLeft" activeCell="N10" activeCellId="0" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -420,6 +420,10 @@
       <c r="M3" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="N3" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -461,6 +465,10 @@
       <c r="M4" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="N4" s="1" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -503,6 +511,10 @@
       <c r="M5" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="N5" s="1" t="n">
+        <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -545,6 +557,10 @@
       <c r="M6" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="N6" s="1" t="n">
+        <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -587,6 +603,10 @@
       <c r="M7" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="N7" s="1" t="n">
+        <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -629,6 +649,10 @@
       <c r="M8" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="N8" s="1" t="n">
+        <f aca="false">10/12</f>
+        <v>0.833333333333333</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
@@ -671,6 +695,10 @@
       <c r="M9" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="N9" s="1" t="n">
+        <f aca="false">11/12</f>
+        <v>0.916666666666667</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -755,6 +783,10 @@
       <c r="M12" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="N12" s="1" t="n">
+        <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -797,6 +829,10 @@
       <c r="M13" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="N13" s="1" t="n">
+        <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
@@ -839,6 +875,10 @@
       <c r="M14" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="N14" s="1" t="n">
+        <f aca="false">10.5/12</f>
+        <v>0.875</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
@@ -881,6 +921,10 @@
       <c r="M15" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="N15" s="1" t="n">
+        <f aca="false">10.5/12</f>
+        <v>0.875</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
@@ -923,6 +967,10 @@
       <c r="M16" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="N16" s="1" t="n">
+        <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
@@ -965,6 +1013,10 @@
       <c r="M17" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="N17" s="1" t="n">
+        <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
@@ -1003,6 +1055,10 @@
       <c r="M18" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="N18" s="1" t="n">
+        <f aca="false">12/12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -1043,6 +1099,10 @@
         <v>1</v>
       </c>
       <c r="M19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N19" s="1" t="n">
+        <f aca="false">12/12</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
final lecture and refraction law lab update
</commit_message>
<xml_diff>
--- a/Semester2/grades/Grades.xlsx
+++ b/Semester2/grades/Grades.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t xml:space="preserve">First name</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">Midterm 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final Project Presentation</t>
   </si>
   <si>
     <t xml:space="preserve">Susana</t>
@@ -311,10 +314,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N10" activeCellId="0" sqref="N10"/>
+      <selection pane="topLeft" activeCell="P11" activeCellId="0" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -333,7 +336,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="21.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.39"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="16" style="1" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="25.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="17" style="1" width="8.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -378,16 +382,19 @@
       <c r="O2" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="P2" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="1" t="n">
         <f aca="false">10.5/10</f>
@@ -427,13 +434,13 @@
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="1" t="n">
         <f aca="false">0</f>
@@ -472,13 +479,13 @@
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="n">
         <f aca="false">9.25/10</f>
@@ -518,13 +525,13 @@
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -564,13 +571,13 @@
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -610,13 +617,13 @@
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F8" s="1" t="n">
         <f aca="false">8/10</f>
@@ -656,13 +663,13 @@
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F9" s="1" t="n">
         <f aca="false">8/10</f>
@@ -702,13 +709,13 @@
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F11" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -741,16 +748,20 @@
       <c r="M11" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="P11" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F12" s="1" t="n">
         <f aca="false">8.5/10</f>
@@ -790,13 +801,13 @@
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F13" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -833,16 +844,20 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="P13" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F14" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -882,13 +897,13 @@
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F15" s="1" t="n">
         <f aca="false">9.75/10</f>
@@ -928,13 +943,13 @@
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F16" s="1" t="n">
         <f aca="false">9/10</f>
@@ -974,13 +989,13 @@
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F17" s="1" t="n">
         <f aca="false">9/10</f>
@@ -1020,13 +1035,13 @@
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F18" s="1" t="n">
         <f aca="false">9.5/10</f>
@@ -1059,16 +1074,20 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="P18" s="1" t="n">
+        <f aca="false">1</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F19" s="1" t="n">
         <f aca="false">9/10</f>

</xml_diff>

<commit_message>
finished grading midterm 2
</commit_message>
<xml_diff>
--- a/Semester2/grades/Grades.xlsx
+++ b/Semester2/grades/Grades.xlsx
@@ -317,7 +317,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O7" activeCellId="0" sqref="O7"/>
+      <selection pane="topLeft" activeCell="O10" activeCellId="0" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -548,6 +548,10 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="O5" s="1" t="n">
+        <f aca="false">46/60</f>
+        <v>0.766666666666667</v>
+      </c>
       <c r="P5" s="1" t="n">
         <v>1</v>
       </c>
@@ -601,6 +605,10 @@
         <f aca="false">12/12</f>
         <v>1</v>
       </c>
+      <c r="O6" s="1" t="n">
+        <f aca="false">55/60</f>
+        <v>0.916666666666667</v>
+      </c>
       <c r="P6" s="1" t="n">
         <v>1</v>
       </c>
@@ -767,6 +775,10 @@
       <c r="N9" s="1" t="n">
         <f aca="false">11/12</f>
         <v>0.916666666666667</v>
+      </c>
+      <c r="O9" s="1" t="n">
+        <f aca="false">54.5/60</f>
+        <v>0.908333333333333</v>
       </c>
       <c r="P9" s="1" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
grade update - midterm 2
</commit_message>
<xml_diff>
--- a/Semester2/grades/Grades.xlsx
+++ b/Semester2/grades/Grades.xlsx
@@ -317,7 +317,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O10" activeCellId="0" sqref="O10"/>
+      <selection pane="topLeft" activeCell="N12" activeCellId="0" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -333,10 +333,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="21.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="20.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="25.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="20.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="17.56"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="18" style="1" width="8.5"/>
   </cols>
@@ -828,6 +828,10 @@
       </c>
       <c r="M11" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="N11" s="1" t="n">
+        <f aca="false">11/12</f>
+        <v>0.916666666666667</v>
       </c>
       <c r="O11" s="1" t="n">
         <f aca="false">51/60</f>

</xml_diff>